<commit_message>
CP-35: For question "what did you not need to order?" bold and underline "not"
- Capitalize "not" instead
</commit_message>
<xml_diff>
--- a/resources/vocabulary-source-generation/src/main/resources/Care_Pathway_Data_Elements.xlsx
+++ b/resources/vocabulary-source-generation/src/main/resources/Care_Pathway_Data_Elements.xlsx
@@ -402,7 +402,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">not</t>
+      <t xml:space="preserve">NOT</t>
     </r>
     <r>
       <rPr>
@@ -2271,7 +2271,7 @@
   <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A44" activeCellId="0" sqref="A44"/>
+      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3495,8 +3495,8 @@
   </sheetPr>
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C73" activeCellId="0" sqref="C73"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A79" activeCellId="0" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>